<commit_message>
feat: add insert record function for inesrting the updates
</commit_message>
<xml_diff>
--- a/covinfinity-dataset.xlsx
+++ b/covinfinity-dataset.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\rag-chatbot\rag-chatbot-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125D33F8-D1DC-40EE-867A-0060C668A4E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29F6D47-E60B-40D3-92C9-2A94E7932A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -404,15 +404,15 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" customWidth="1"/>
-    <col min="3" max="3" width="44.33203125" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
fix: insert vector into db successfully done
</commit_message>
<xml_diff>
--- a/covinfinity-dataset.xlsx
+++ b/covinfinity-dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\rag-chatbot\rag-chatbot-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29F6D47-E60B-40D3-92C9-2A94E7932A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D21531-E62A-4DD0-AEE7-C9B5CC8B428C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
-    <t>ConversationID</t>
-  </si>
-  <si>
     <t>Role</t>
   </si>
   <si>
@@ -70,6 +67,9 @@
   </si>
   <si>
     <t>Typically 3–4 weeks, depending on features and revisions.</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -404,7 +404,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -415,18 +415,18 @@
     <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -434,13 +434,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -448,13 +448,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -462,13 +462,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -476,13 +476,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -490,13 +490,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -504,13 +504,13 @@
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: vector search and implementation complete
</commit_message>
<xml_diff>
--- a/covinfinity-dataset.xlsx
+++ b/covinfinity-dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\rag-chatbot\rag-chatbot-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D21531-E62A-4DD0-AEE7-C9B5CC8B428C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB07672-FC45-4E95-8B1B-1D2593D2B6C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -403,8 +403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>